<commit_message>
update on modal window
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_(Rajesh.S).xlsx
+++ b/Wave 5_React_Tracker_(Rajesh.S).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Git URL:</t>
   </si>
   <si>
-    <t>23/08/2016</t>
-  </si>
-  <si>
     <t>Labels</t>
   </si>
   <si>
@@ -75,10 +72,7 @@
     <t>25/08/2016</t>
   </si>
   <si>
-    <t>Data is fetching</t>
-  </si>
-  <si>
-    <t>In Progress</t>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -410,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -418,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -468,10 +462,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>6</v>
@@ -491,78 +485,40 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="K4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="L4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Up to Router with sent, inbox, compose
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_(Rajesh.S).xlsx
+++ b/Wave 5_React_Tracker_(Rajesh.S).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -66,13 +66,10 @@
     <t>Done</t>
   </si>
   <si>
-    <t>TD</t>
-  </si>
-  <si>
-    <t>25/08/2016</t>
-  </si>
-  <si>
-    <t>In progress</t>
+    <t>29/08/2016</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -404,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -485,40 +482,40 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>